<commit_message>
committing encapsulation slides (missing notes still)
</commit_message>
<xml_diff>
--- a/misused-and-misunderstood-apis/src/main/resources/stats-processed-scrubbed.xlsx
+++ b/misused-and-misunderstood-apis/src/main/resources/stats-processed-scrubbed.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\installs\workspaces\devcon\growth-in-code-presentation\misused-and-misunderstood-apis\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stats-processed" sheetId="1" r:id="rId1"/>
     <sheet name="class-info-per-year" sheetId="3" r:id="rId2"/>
     <sheet name="release-per-year" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -3694,11 +3694,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -3708,11 +3707,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Class</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Growth Per Year</a:t>
+              <a:t>Class A Growth Per Year</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3730,11 +3725,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -3767,45 +3761,49 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="15000"/>
+                        <a:lumOff val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3825,16 +3823,25 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="ellipse">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -3936,45 +3943,49 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="15000"/>
+                        <a:lumOff val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -3994,16 +4005,25 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="ellipse">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -4105,45 +4125,49 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="15000"/>
+                        <a:lumOff val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4163,16 +4187,25 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="ellipse">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -4274,45 +4307,49 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="31750" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent6">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1"/>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="15000"/>
+                        <a:lumOff val="85000"/>
+                      </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -4332,16 +4369,25 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="ellipse">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
                     <a:ln w="9525">
                       <a:solidFill>
-                        <a:schemeClr val="dk1">
+                        <a:schemeClr val="lt1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -4437,7 +4483,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="589971256"/>
         <c:axId val="589971584"/>
@@ -4465,13 +4510,19 @@
                   </c:strRef>
                 </c:tx>
                 <c:spPr>
-                  <a:ln w="31750" cap="rnd">
+                  <a:ln w="22225" cap="rnd">
                     <a:solidFill>
                       <a:schemeClr val="accent2"/>
                     </a:solidFill>
-                    <a:round/>
                   </a:ln>
-                  <a:effectLst/>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent2">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
                 </c:spPr>
                 <c:marker>
                   <c:symbol val="none"/>
@@ -4491,9 +4542,11 @@
                     <a:lstStyle/>
                     <a:p>
                       <a:pPr>
-                        <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                           <a:solidFill>
-                            <a:schemeClr val="lt1"/>
+                            <a:schemeClr val="lt1">
+                              <a:lumMod val="75000"/>
+                            </a:schemeClr>
                           </a:solidFill>
                           <a:latin typeface="+mn-lt"/>
                           <a:ea typeface="+mn-ea"/>
@@ -4518,11 +4571,11 @@
                         <c:spPr>
                           <a:ln w="9525">
                             <a:solidFill>
-                              <a:schemeClr val="dk1">
+                              <a:schemeClr val="lt1">
                                 <a:lumMod val="50000"/>
-                                <a:lumOff val="50000"/>
                               </a:schemeClr>
                             </a:solidFill>
+                            <a:round/>
                           </a:ln>
                           <a:effectLst/>
                         </c:spPr>
@@ -4632,20 +4685,39 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -4654,11 +4726,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4681,7 +4752,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -4690,15 +4761,14 @@
                 <a:gsLst>
                   <a:gs pos="100000">
                     <a:schemeClr val="dk1">
-                      <a:lumMod val="95000"/>
-                      <a:lumOff val="5000"/>
-                      <a:alpha val="42000"/>
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
                     </a:schemeClr>
                   </a:gs>
                   <a:gs pos="0">
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                      <a:alpha val="36000"/>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:gs>
                 </a:gsLst>
@@ -4713,6 +4783,32 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:crossAx val="589971256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
@@ -4726,15 +4822,10 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -4747,9 +4838,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
+                <a:schemeClr val="lt1">
                   <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -4766,30 +4856,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:round/>
@@ -4821,10 +4898,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="103"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="3"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -4835,11 +4912,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -4849,11 +4925,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Releases</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> By Year for Project Containing Class</a:t>
+              <a:t>Releases By Year for Project Containing Class A</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4871,11 +4943,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -4909,15 +4980,79 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>'release-per-year'!$B$1:$J$1</c:f>
@@ -4996,15 +5131,16 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
         <c:axId val="416524048"/>
         <c:axId val="416520440"/>
       </c:barChart>
@@ -5015,20 +5151,92 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -5039,9 +5247,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5069,17 +5276,81 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Releases</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5098,9 +5369,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -5129,11 +5399,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -5241,42 +5514,8 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
   <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -5797,15 +6036,14 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" b="1" kern="1200"/>
@@ -5815,23 +6053,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea>
     <cs:lnRef idx="0"/>
@@ -5841,30 +6067,17 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="39000">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5874,120 +6087,156 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
           <a:lumMod val="65000"/>
           <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
         </a:schemeClr>
       </a:solidFill>
     </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
           </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -6011,17 +6260,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -6033,7 +6281,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -6045,10 +6293,10 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6062,12 +6310,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -6081,9 +6328,8 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6111,15 +6357,14 @@
           <a:gsLst>
             <a:gs pos="100000">
               <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -6137,25 +6382,27 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:gradFill>
           <a:gsLst>
             <a:gs pos="100000">
               <a:schemeClr val="dk1">
-                <a:lumMod val="95000"/>
-                <a:lumOff val="5000"/>
-                <a:alpha val="42000"/>
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="0">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="75000"/>
-                <a:alpha val="36000"/>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -6169,12 +6416,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="dash"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -6188,11 +6434,11 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -6201,19 +6447,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="95000"/>
-          <a:alpha val="39000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
   <cs:plotArea>
@@ -6237,22 +6474,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -6265,9 +6490,8 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6279,12 +6503,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -6293,12 +6516,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -6308,9 +6533,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6324,15 +6548,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6341,16 +6567,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6365,33 +6585,46 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -6400,38 +6633,14 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6441,23 +6650,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -6465,71 +6669,131 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6545,21 +6809,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6569,22 +6830,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -6593,14 +6854,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6612,14 +6872,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6631,30 +6890,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -6664,16 +6928,29 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -6683,14 +6960,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6702,14 +6978,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6721,27 +6996,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -6749,9 +7023,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6761,14 +7034,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -6780,12 +7052,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -6794,14 +7065,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -6810,9 +7082,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6826,15 +7097,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -6843,9 +7116,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -6855,14 +7127,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -6906,16 +7172,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6942,15 +7208,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7271,8 +7537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10258,8 +10524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10545,7 +10811,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>